<commit_message>
add next key test
</commit_message>
<xml_diff>
--- a/resource/PhantomRead/PhantomRead.xlsx
+++ b/resource/PhantomRead/PhantomRead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyBox\Github\GitDisk\resource\PhantomRead\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F49F4F-589A-48B1-97CD-4A111A699A24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E097888F-03A4-432A-9826-A666823AE5C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="55">
   <si>
     <t>隔离级别</t>
   </si>
@@ -239,12 +239,30 @@
   <si>
     <t>数据行号</t>
   </si>
+  <si>
+    <t>读提交隔离级别</t>
+  </si>
+  <si>
+    <t>可重复读隔离级别</t>
+  </si>
+  <si>
+    <t>update users set name='Jonny' where class_id=1</t>
+  </si>
+  <si>
+    <t>Jonny</t>
+  </si>
+  <si>
+    <t>waiting ….</t>
+  </si>
+  <si>
+    <t>事务1提交后,事务B的insert才执行</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +311,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,14 +600,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -630,6 +656,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,7 +686,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -669,7 +698,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -688,6 +717,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -697,54 +729,254 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="注释" xfId="4" builtinId="10"/>
+    <cellStyle name="注释" xfId="5" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="4" builtinId="11"/>
     <cellStyle name="输入" xfId="3" builtinId="20"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1833,107 +2065,131 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D6293AD-A75E-4F6C-A027-B417F067461A}" name="表2" displayName="表2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" headerRowCellStyle="好">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D6293AD-A75E-4F6C-A027-B417F067461A}" name="表2" displayName="表2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" headerRowCellStyle="好">
   <autoFilter ref="A1:D5" xr:uid="{97F19234-BE1F-45FF-A6F6-2E59BC65D2AE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5373A9E3-C53F-445B-ABA6-62F507808B52}" name="隔离级别" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{ABA8823C-A40C-4703-88F3-3E24A6A07C0C}" name="脏读（Dirty Read）" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{D4B41ADD-8C13-44D5-8426-C872A32E160B}" name="不可重复读（NonRepeatable Read）" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{10DD6242-F7F9-4910-9712-6B9FC58F0D21}" name="幻读（Phantom Read）" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{5373A9E3-C53F-445B-ABA6-62F507808B52}" name="隔离级别" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{ABA8823C-A40C-4703-88F3-3E24A6A07C0C}" name="脏读（Dirty Read）" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{D4B41ADD-8C13-44D5-8426-C872A32E160B}" name="不可重复读（NonRepeatable Read）" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{10DD6242-F7F9-4910-9712-6B9FC58F0D21}" name="幻读（Phantom Read）" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{CF30430F-1173-4253-8A85-17D34D8BC874}" name="表3_815" displayName="表3_815" ref="A14:C17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="注释">
+  <autoFilter ref="A14:C17" xr:uid="{D1342F62-CE27-42CE-BA24-323BBE7BBF7B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5B222368-219D-4656-BB51-0F3FFCF8201C}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{20A6E00E-A344-4863-A3AF-E32DFA9D2ABC}" name="name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B82D8D42-A999-4668-9CFF-6B6CD5E383CC}" name="class_id" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1D240C43-548B-4591-A1F4-BFD3EF8DA339}" name="表3_81516" displayName="表3_81516" ref="A33:C36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="注释">
+  <autoFilter ref="A33:C36" xr:uid="{78431AAD-3F7A-47F4-9806-70BA3CEB0ED9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BE106B84-8F9E-4778-9C57-8CFC932B9BB3}" name="id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{42667040-18BE-484B-B10C-E11F71995C5A}" name="name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{474C80F2-4C74-4FBE-842D-FEEEE6572021}" name="class_id" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40564FB3-9926-40FA-9498-D355D24345E3}" name="表3" displayName="表3" ref="F1:H3" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" headerRowCellStyle="好">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40564FB3-9926-40FA-9498-D355D24345E3}" name="表3" displayName="表3" ref="F1:H3" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" headerRowCellStyle="好">
   <autoFilter ref="F1:H3" xr:uid="{706CDEE7-74D5-4831-83BF-E47D9053969D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E03B532-84E0-4CCE-8FEF-B1CCC0959555}" name="id" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{24811457-580F-4BEA-B7D1-63D03B5880F4}" name="name" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{3E19F4AF-670E-4F8F-903C-66B4D7B451A3}" name="class_id" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{4E03B532-84E0-4CCE-8FEF-B1CCC0959555}" name="id" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{24811457-580F-4BEA-B7D1-63D03B5880F4}" name="name" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{3E19F4AF-670E-4F8F-903C-66B4D7B451A3}" name="class_id" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A547CD9F-11AF-4BC3-B7F2-B685C62DF31D}" name="表4" displayName="表4" ref="A1:B11" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" headerRowCellStyle="好">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A547CD9F-11AF-4BC3-B7F2-B685C62DF31D}" name="表4" displayName="表4" ref="A1:B11" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" headerRowCellStyle="好">
   <autoFilter ref="A1:B11" xr:uid="{09BB5791-43CA-4081-A658-BCCE5A71ADB0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5A905238-6B35-4ABA-9187-3D7F93F0D48F}" name="事务 1" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{4CFED88F-B827-4F54-ACD7-BBA1CA426BAC}" name="事务 2" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{5A905238-6B35-4ABA-9187-3D7F93F0D48F}" name="事务 1" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{4CFED88F-B827-4F54-ACD7-BBA1CA426BAC}" name="事务 2" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9B6A69A7-054B-42D7-A92E-D833A9026D8F}" name="表5" displayName="表5" ref="A2:B12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" headerRowCellStyle="好">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9B6A69A7-054B-42D7-A92E-D833A9026D8F}" name="表5" displayName="表5" ref="A2:B12" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" headerRowCellStyle="好">
   <autoFilter ref="A2:B12" xr:uid="{7789C5F8-21FA-4B15-B3E6-3B6F950FE54B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{82FF0183-D146-4852-A21A-8AFDEC5C9091}" name="事务 1" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{E58A7DF5-ADD7-4E4C-AC3E-EBBDE43B76F1}" name="事务 2" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{82FF0183-D146-4852-A21A-8AFDEC5C9091}" name="事务 1" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{E58A7DF5-ADD7-4E4C-AC3E-EBBDE43B76F1}" name="事务 2" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DA47CA3B-20BC-4196-BA6C-82CE7888D9CD}" name="表3_8" displayName="表3_8" ref="A13:C16" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" headerRowCellStyle="注释">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DA47CA3B-20BC-4196-BA6C-82CE7888D9CD}" name="表3_8" displayName="表3_8" ref="A13:C16" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" headerRowCellStyle="注释">
   <autoFilter ref="A13:C16" xr:uid="{7D2D1BB2-3740-4AD1-ABAC-E57B64B3B43E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{867596D8-7BD8-4255-B3B7-7486A750217E}" name="id" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{FE7F2DC3-96CD-4790-8A60-3971EB042CE7}" name="name" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{4923B8C0-BFEB-4C96-8862-4C0678C1FB92}" name="class_id" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{867596D8-7BD8-4255-B3B7-7486A750217E}" name="id" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{FE7F2DC3-96CD-4790-8A60-3971EB042CE7}" name="name" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{4923B8C0-BFEB-4C96-8862-4C0678C1FB92}" name="class_id" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FCE63FFF-3D84-42E1-9EDB-513FBBC569E4}" name="表12" displayName="表12" ref="A4:C6" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25" tableBorderDxfId="29" totalsRowBorderDxfId="32" headerRowCellStyle="注释">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FCE63FFF-3D84-42E1-9EDB-513FBBC569E4}" name="表12" displayName="表12" ref="A4:C6" totalsRowShown="0" headerRowDxfId="34" dataDxfId="35" tableBorderDxfId="39" totalsRowBorderDxfId="42" headerRowCellStyle="注释">
   <autoFilter ref="A4:C6" xr:uid="{6FF22E54-6FB1-422F-A7E7-7F7D4DC17395}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{09F700CA-7719-4C66-8C06-743CBC023729}" name="id" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{09CA90D6-75D4-427D-9F70-F3A04FE1D4BA}" name="name" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{7F3766BF-86B5-4358-B556-7392EC967969}" name="class_id" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{09F700CA-7719-4C66-8C06-743CBC023729}" name="id" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{09CA90D6-75D4-427D-9F70-F3A04FE1D4BA}" name="name" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{7F3766BF-86B5-4358-B556-7392EC967969}" name="class_id" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B69A9A21-32F5-4DC8-94E4-F3F32CE23085}" name="表13" displayName="表13" ref="A12:C14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19" tableBorderDxfId="23" totalsRowBorderDxfId="30" headerRowCellStyle="注释">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B69A9A21-32F5-4DC8-94E4-F3F32CE23085}" name="表13" displayName="表13" ref="A12:C14" totalsRowShown="0" headerRowDxfId="28" dataDxfId="29" tableBorderDxfId="33" totalsRowBorderDxfId="40" headerRowCellStyle="注释">
   <autoFilter ref="A12:C14" xr:uid="{3AD65E3D-92A6-493B-A090-7BB7F952B1A2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0DECEEC2-8B96-4AD1-A4BE-915970B356B4}" name="id" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{4664AF7A-5543-42E6-B76D-76E04B915F44}" name="name" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{07F877D1-E7F4-43F1-AD0F-25CDE608649D}" name="class_id" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{0DECEEC2-8B96-4AD1-A4BE-915970B356B4}" name="id" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{4664AF7A-5543-42E6-B76D-76E04B915F44}" name="name" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{07F877D1-E7F4-43F1-AD0F-25CDE608649D}" name="class_id" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CA288364-29FB-4C37-B691-C0104A43E1BD}" name="表12_11" displayName="表12_11" ref="E10:G12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CA288364-29FB-4C37-B691-C0104A43E1BD}" name="表12_11" displayName="表12_11" ref="E10:G12" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="26">
   <autoFilter ref="E10:G12" xr:uid="{05647586-9970-47D7-A8DD-02C72520F878}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{108E5160-2B1A-464D-AB42-206C55C8A0AD}" name="id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F64EECDC-388A-41A3-8F24-D24953C44541}" name="name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D606F162-389F-4A3E-945A-9A4CC6AB1D36}" name="class_id" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{108E5160-2B1A-464D-AB42-206C55C8A0AD}" name="id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{F64EECDC-388A-41A3-8F24-D24953C44541}" name="name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{D606F162-389F-4A3E-945A-9A4CC6AB1D36}" name="class_id" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5F888095-F25A-4129-A463-E3F1B99FF4EF}" name="表13_12" displayName="表13_12" ref="E18:G20" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5F888095-F25A-4129-A463-E3F1B99FF4EF}" name="表13_12" displayName="表13_12" ref="E18:G20" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="24">
   <autoFilter ref="E18:G20" xr:uid="{71A85346-D5F3-4A0F-82E5-F299A87A3900}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A09F8D93-C53D-4806-BE43-4FE5691465F2}" name="id" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{380E7136-AB15-4703-8784-04E86B881EFE}" name="name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{DC0A4E70-4E4D-43EF-84DF-69E0218293C9}" name="class_id" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{A09F8D93-C53D-4806-BE43-4FE5691465F2}" name="id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{380E7136-AB15-4703-8784-04E86B881EFE}" name="name" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{DC0A4E70-4E4D-43EF-84DF-69E0218293C9}" name="class_id" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2205,7 +2461,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,25 +2475,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="36" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2339,10 +2595,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2419,7 +2675,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,10 +2689,10 @@
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2512,7 +2768,7 @@
   <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A2" sqref="A2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,12 +2780,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2550,37 +2806,37 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="22">
         <v>1</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>1</v>
       </c>
       <c r="D7" s="5"/>
@@ -2626,13 +2882,13 @@
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="5"/>
@@ -2693,7 +2949,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,15 +2962,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2741,39 +2997,39 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="21">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="21">
         <v>2</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="21">
         <v>1</v>
       </c>
       <c r="D6" s="6"/>
@@ -2825,39 +3081,39 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="A13" s="21">
         <v>1</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="21">
         <v>1</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="21">
         <v>2</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="21">
         <v>1</v>
       </c>
       <c r="D14" s="6"/>
@@ -2912,7 +3168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBFF9E4-B366-4FD3-AB2C-945D7B7BFCEC}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2920,148 +3178,148 @@
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="36"/>
+    <col min="5" max="7" width="9.140625" style="37"/>
     <col min="11" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="24">
+      <c r="B1" s="25">
         <v>1000</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="54">
         <v>1</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>1</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24">
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="24">
         <v>2</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="52">
+      <c r="A4" s="54">
         <v>2</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="24">
         <v>2</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+      <c r="A5" s="54">
         <v>3</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24">
         <v>3</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="24">
         <v>1</v>
       </c>
     </row>
@@ -3071,54 +3329,54 @@
       <c r="G6"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="23" t="s">
         <v>24</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="23" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="23" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="23" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="23" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="22" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="23" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="13"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="22"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="13"/>
       <c r="M9" s="14"/>
     </row>
@@ -3126,16 +3384,16 @@
       <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="22"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="13"/>
       <c r="M10" s="14"/>
     </row>
@@ -3143,16 +3401,16 @@
       <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="19">
         <v>1</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="22"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="13"/>
       <c r="M11" s="14"/>
     </row>
@@ -3160,141 +3418,141 @@
       <c r="E12" s="11">
         <v>2</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="18">
         <v>1</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="22"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="13"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="23" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="22"/>
+      <c r="K13" s="23"/>
       <c r="L13" s="13"/>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="E14" s="22"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="23" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
-      <c r="K14" s="22"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="13"/>
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="22"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="22" t="s">
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="L15" s="13"/>
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="22"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="22" t="s">
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="23" t="s">
         <v>27</v>
       </c>
       <c r="L16" s="13"/>
       <c r="M16" s="14"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="22" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="23" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="40" t="s">
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="42"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="44"/>
     </row>
     <row r="18" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="23"/>
       <c r="I18" s="13"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="47"/>
     </row>
     <row r="19" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="19">
         <v>1</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="23"/>
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="50"/>
     </row>
     <row r="20" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E20" s="11">
         <v>2</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="18">
         <v>1</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="22"/>
+      <c r="K20" s="23"/>
       <c r="L20" s="13"/>
       <c r="M20" s="14"/>
     </row>
@@ -4025,14 +4283,383 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E3B82-074F-4A72-AC2B-F5C98362B2E3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="43.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>1</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>2</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A8:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>